<commit_message>
Cheanges in preview removed: alert
</commit_message>
<xml_diff>
--- a/ad_warn_data/Aerodrome_Warnings_Table.xlsx
+++ b/ad_warn_data/Aerodrome_Warnings_Table.xlsx
@@ -523,7 +523,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">

</xml_diff>